<commit_message>
minor changes and started ReadMe
</commit_message>
<xml_diff>
--- a/docs/test cases.xlsx
+++ b/docs/test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunda\Documents\Universidad\Adidas\PetStoreTestSuite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F09BEB-E117-4409-974F-19B86B604298}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB036CC6-2E02-40EB-964C-5CCF95F62DBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D60B0FB-2937-4D65-8E0B-4CECE67EFFB6}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>1. Send delete order request</t>
   </si>
   <si>
-    <t>queryNonExistenOrder</t>
-  </si>
-  <si>
     <t>1. The order does not exist
 2. The query id is valid</t>
   </si>
@@ -177,9 +174,6 @@
 3. The value for each status is equal to the previous value plus the number of pets added with said status</t>
   </si>
   <si>
-    <t>createOrderWithNegativeQuantity</t>
-  </si>
-  <si>
     <t>1. The pet already exists.
 2. The quantity is a negative value.
 3. The rest of the data is valid</t>
@@ -188,9 +182,6 @@
     <t>Logic/Negative</t>
   </si>
   <si>
-    <t>createOrderWithInvalidId</t>
-  </si>
-  <si>
     <t>1. The pet already exists.
 2. The id is not a number.
 3. The rest of the data is correct</t>
@@ -234,6 +225,15 @@
   </si>
   <si>
     <t>decreaseInventoryStatus</t>
+  </si>
+  <si>
+    <t>queryNonExistentOrder</t>
+  </si>
+  <si>
+    <t>postOrderWithNegativeQuantity</t>
+  </si>
+  <si>
+    <t>postOrderWithInvalidId</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -637,10 +637,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -654,10 +654,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -671,10 +671,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -682,16 +682,16 @@
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -699,47 +699,47 @@
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -747,16 +747,16 @@
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
@@ -764,16 +764,16 @@
     </row>
     <row r="10" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
@@ -781,67 +781,67 @@
     </row>
     <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -849,16 +849,16 @@
     </row>
     <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>
@@ -866,16 +866,16 @@
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Bugs fixed, new test cases added
</commit_message>
<xml_diff>
--- a/docs/test cases.xlsx
+++ b/docs/test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunda\Documents\Universidad\Adidas\PetStoreTestSuite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395B2782-6781-4192-B76A-16B8B3AD72B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CDB3F9-F8D0-43AF-8A87-2DD020A86042}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D60B0FB-2937-4D65-8E0B-4CECE67EFFB6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>Test Case</t>
   </si>
@@ -183,10 +183,6 @@
     <t>getOrderWithInvalidId</t>
   </si>
   <si>
-    <t>1. The order already exists.
-2. The query id is not valid</t>
-  </si>
-  <si>
     <t>1. Error 400 invalid id supplied is received</t>
   </si>
   <si>
@@ -316,6 +312,60 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>deleteOrderWithInvalidId</t>
+  </si>
+  <si>
+    <t>1. The query id is not valid</t>
+  </si>
+  <si>
+    <t>1. The input id is invalid</t>
+  </si>
+  <si>
+    <t>validateInventoryWithPetChange</t>
+  </si>
+  <si>
+    <t>1. A pet already exists in the system
+2. The inventory status is known</t>
+  </si>
+  <si>
+    <t>According to the service contract if an invalid id is supplied, an error with status code 400 should be received.</t>
+  </si>
+  <si>
+    <t>1. Update pet status using the form function.
+2 Query the inventory.</t>
+  </si>
+  <si>
+    <t>3. The old status should decrease by one, and the new status should increase by one.</t>
+  </si>
+  <si>
+    <t>Inventory should keep a correct track of the different status when pets change.</t>
+  </si>
+  <si>
+    <t>createOrderWithInvalidQuantity</t>
+  </si>
+  <si>
+    <t>1. The pet already exists.
+2. The order quantity is a Long number.</t>
+  </si>
+  <si>
+    <t>1. Send post order request.</t>
+  </si>
+  <si>
+    <t>1. Error 400 invalid order is received.</t>
+  </si>
+  <si>
+    <t>The value shouldn't cause a crash in the system. Incorrect input should be handled.</t>
   </si>
 </sst>
 </file>
@@ -700,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4026A7-B744-4E85-9FCF-F217023FAEC8}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,9 +764,10 @@
     <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,13 +784,16 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -756,13 +810,16 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H2" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -779,13 +836,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H3" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -802,15 +862,18 @@
         <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H4" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -825,13 +888,16 @@
         <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H5" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -848,13 +914,16 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H6" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -871,13 +940,16 @@
         <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -894,13 +966,16 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H8" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -911,19 +986,22 @@
         <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="G9" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="H9" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -940,15 +1018,18 @@
         <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="H10" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>39</v>
@@ -963,15 +1044,18 @@
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H11" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
@@ -983,44 +1067,50 @@
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H12" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H13" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1032,67 +1122,76 @@
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G15" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H15" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="H16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" t="s">
         <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
@@ -1101,33 +1200,114 @@
         <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H17" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" s="4">
         <v>2</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>